<commit_message>
update: Programação Linear Inteira
</commit_message>
<xml_diff>
--- a/09-Programacao-Linear-Inteira/Book1.xlsx
+++ b/09-Programacao-Linear-Inteira/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cintiashinoda/Desktop/[UTFPR]/utfpr_emma-repo/09-Programacao-Linear-Inteira/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D96DF2-17D9-7742-ABA8-2C68B4BF40BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873123E5-4505-A84E-B776-C516C0CC656B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24020" yWindow="1100" windowWidth="21860" windowHeight="26260" activeTab="3" xr2:uid="{B133C9D0-67B2-C941-B549-F08E9AA8E72F}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'P1-Ex1'!$I$6:$I$8</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">'P1-Ex2'!$I$6:$I$8</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'P1-Ex3'!$I$5:$I$7</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'P1-Ex4'!$I$6:$I$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'P1-Ex4'!$I$6:$I$8</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'P1-Ex1'!$I$6:$I$8</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
@@ -121,7 +121,7 @@
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'P1-Ex1'!$J$6:$J$8</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">'P1-Ex2'!$J$6:$J$8</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'P1-Ex3'!$J$5:$J$7</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'P1-Ex4'!$J$6:$J$7</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'P1-Ex4'!$J$6:$J$8</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'P1-Ex1'!$J$6:$J$8</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="138">
   <si>
     <t>Maximizar z = x1 + 5x2 + 9x3 + 5x4</t>
   </si>
@@ -1158,6 +1158,9 @@
   </si>
   <si>
     <t>Z = 13</t>
+  </si>
+  <si>
+    <t>Solução Candidata</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1449,6 +1452,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2086,7 +2092,7 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="T9" s="36" t="s">
+      <c r="T9" s="37" t="s">
         <v>17</v>
       </c>
       <c r="U9" s="33"/>
@@ -2143,10 +2149,10 @@
       <c r="R17" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="S17" s="35"/>
+      <c r="S17" s="36"/>
     </row>
     <row r="18" spans="5:26">
-      <c r="G18" s="66" t="s">
+      <c r="G18" s="67" t="s">
         <v>15</v>
       </c>
       <c r="R18" s="22" t="s">
@@ -2190,10 +2196,10 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="5:26">
-      <c r="E22" s="66" t="s">
+      <c r="E22" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="66" t="s">
+      <c r="I22" s="67" t="s">
         <v>23</v>
       </c>
       <c r="R22" s="14" t="s">
@@ -2408,7 +2414,7 @@
       <c r="G34" t="s">
         <v>32</v>
       </c>
-      <c r="R34" s="38" t="s">
+      <c r="R34" s="39" t="s">
         <v>56</v>
       </c>
       <c r="S34" s="31"/>
@@ -2607,7 +2613,7 @@
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
-      <c r="P43" s="37" t="s">
+      <c r="P43" s="38" t="s">
         <v>55</v>
       </c>
       <c r="R43" s="30"/>
@@ -3005,43 +3011,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="10.83203125" style="40"/>
-    <col min="11" max="11" width="5.6640625" style="40" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" style="48" customWidth="1"/>
-    <col min="13" max="13" width="2.83203125" style="40" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" style="40" customWidth="1"/>
-    <col min="15" max="15" width="2.83203125" style="40" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" style="48" customWidth="1"/>
-    <col min="17" max="17" width="2.83203125" style="40" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="40" customWidth="1"/>
-    <col min="19" max="19" width="2.83203125" style="40" customWidth="1"/>
-    <col min="20" max="20" width="18.83203125" style="48" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="40"/>
+    <col min="1" max="10" width="10.83203125" style="41"/>
+    <col min="11" max="11" width="5.6640625" style="41" customWidth="1"/>
+    <col min="12" max="12" width="18.83203125" style="49" customWidth="1"/>
+    <col min="13" max="13" width="2.83203125" style="41" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" style="41" customWidth="1"/>
+    <col min="15" max="15" width="2.83203125" style="41" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" style="49" customWidth="1"/>
+    <col min="17" max="17" width="2.83203125" style="41" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" style="41" customWidth="1"/>
+    <col min="19" max="19" width="2.83203125" style="41" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" style="49" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="17" thickBot="1">
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="41">
+      <c r="H1" s="42">
         <f>SUMPRODUCT(E2:H2,E4:H4)</f>
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="41">
         <v>7</v>
       </c>
-      <c r="F2" s="40">
+      <c r="F2" s="41">
         <v>9</v>
       </c>
-      <c r="G2" s="40">
+      <c r="G2" s="41">
         <v>1</v>
       </c>
-      <c r="H2" s="40">
+      <c r="H2" s="41">
         <v>6</v>
       </c>
       <c r="R2" s="24" t="s">
@@ -3049,141 +3055,141 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="R3" s="45" t="s">
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="R3" s="46" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="E4" s="43">
+      <c r="E4" s="44">
         <v>1</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="44">
         <v>2</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="44">
         <v>0</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="44">
         <v>2</v>
       </c>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="R4" s="45" t="s">
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="R4" s="46" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42" t="s">
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="46" t="s">
+      <c r="R5" s="47" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="43">
         <v>8</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="43">
         <v>2</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="43">
         <v>4</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="43">
         <v>2</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="43">
         <f>SUMPRODUCT(E6:H6,E4:H4)</f>
         <v>16</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="43">
         <v>16</v>
       </c>
-      <c r="R6" s="45" t="s">
+      <c r="R6" s="46" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="43">
         <v>4</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="43">
         <v>8</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="43">
         <v>2</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="43">
         <v>0</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="43">
         <f>SUMPRODUCT(E7:H7,E4:H4)</f>
         <v>20</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="43">
         <v>20</v>
       </c>
-      <c r="R7" s="47" t="s">
+      <c r="R7" s="48" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="17" thickBot="1">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="43">
         <v>7</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="43">
         <v>0</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="43">
         <v>6</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="43">
         <v>2</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="43">
         <f>SUMPRODUCT(E8:H8,E4:H4)</f>
         <v>11</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="43">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="41" t="s">
         <v>61</v>
       </c>
       <c r="P9" s="17" t="s">
@@ -3194,58 +3200,58 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="P10" s="49" t="s">
+      <c r="P10" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="T10" s="49" t="s">
+      <c r="T10" s="50" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="P11" s="50" t="s">
+      <c r="P11" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="T11" s="53" t="s">
+      <c r="T11" s="54" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="P12" s="50" t="s">
+      <c r="P12" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="T12" s="53" t="s">
+      <c r="T12" s="54" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="P13" s="50" t="s">
+      <c r="P13" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="T13" s="53" t="s">
+      <c r="T13" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="P14" s="50" t="s">
+      <c r="P14" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="T14" s="53" t="s">
+      <c r="T14" s="54" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="17" thickBot="1">
-      <c r="P15" s="51" t="s">
+      <c r="P15" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="T15" s="54" t="s">
+      <c r="T15" s="55" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="17" thickBot="1">
-      <c r="T16" s="52" t="s">
+      <c r="T16" s="53" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3258,63 +3264,63 @@
       </c>
     </row>
     <row r="18" spans="8:16">
-      <c r="N18" s="55" t="s">
+      <c r="N18" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="P18" s="55" t="s">
+      <c r="P18" s="56" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="8:16">
-      <c r="N19" s="50" t="s">
+      <c r="N19" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="P19" s="53" t="s">
+      <c r="P19" s="54" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="8:16">
-      <c r="N20" s="50" t="s">
+      <c r="N20" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="P20" s="53" t="s">
+      <c r="P20" s="54" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="21" spans="8:16">
-      <c r="N21" s="56" t="s">
+      <c r="N21" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="P21" s="53" t="s">
+      <c r="P21" s="54" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="8:16">
-      <c r="N22" s="50" t="s">
+      <c r="N22" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="P22" s="53" t="s">
+      <c r="P22" s="54" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="8:16">
-      <c r="N23" s="50" t="s">
+      <c r="N23" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="P23" s="53" t="s">
+      <c r="P23" s="54" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="8:16" ht="17" thickBot="1">
-      <c r="N24" s="57" t="s">
+      <c r="N24" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="P24" s="54" t="s">
+      <c r="P24" s="55" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="25" spans="8:16">
-      <c r="P25" s="52" t="s">
+      <c r="P25" s="53" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3323,88 +3329,88 @@
       <c r="L27" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="N27" s="63" t="s">
+      <c r="N27" s="64" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="8:16">
-      <c r="L28" s="56" t="s">
+      <c r="L28" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="N28" s="60" t="s">
+      <c r="N28" s="61" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="8:16">
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="58" t="s">
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="N29" s="61" t="s">
+      <c r="N29" s="62" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="30" spans="8:16">
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="58" t="s">
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="N30" s="61" t="s">
+      <c r="N30" s="62" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="31" spans="8:16">
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="58" t="s">
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="N31" s="61" t="s">
+      <c r="N31" s="62" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="8:16">
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="58" t="s">
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="61" t="s">
+      <c r="N32" s="62" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="8:14">
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="58" t="s">
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="N33" s="61" t="s">
+      <c r="N33" s="62" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="8:14" ht="17" thickBot="1">
-      <c r="L34" s="59" t="s">
+      <c r="L34" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="N34" s="62" t="s">
+      <c r="N34" s="63" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="35" spans="8:14">
-      <c r="N35" s="65" t="s">
+      <c r="N35" s="66" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3439,51 +3445,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="17" thickBot="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="I1" s="40" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="I1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="41">
+      <c r="J1" s="42">
         <f>SUMPRODUCT(E2:G2,E4:G4)</f>
         <v>18.5</v>
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="E2" s="40">
+      <c r="E2" s="41">
         <v>3</v>
       </c>
-      <c r="F2" s="40">
+      <c r="F2" s="41">
         <v>4</v>
       </c>
-      <c r="G2" s="40">
+      <c r="G2" s="41">
         <v>3</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
       <c r="R2" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:22">
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="64"/>
-      <c r="I3" s="42" t="s">
+      <c r="H3" s="65"/>
+      <c r="I3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="43" t="s">
         <v>12</v>
       </c>
       <c r="R3" s="18" t="s">
@@ -3494,41 +3500,41 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="44">
         <v>3.5</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="44">
         <v>2</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="44">
         <v>0</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
       <c r="R4" s="21" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="43">
         <v>3</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="43">
         <v>2</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="43">
         <v>2</v>
       </c>
-      <c r="H5" s="64"/>
+      <c r="H5" s="65"/>
       <c r="I5" s="9">
         <f>SUMPRODUCT(E5:G5,E4:G4)</f>
         <v>14.5</v>
       </c>
-      <c r="J5" s="64">
+      <c r="J5" s="65">
         <v>13</v>
       </c>
       <c r="R5" s="18" t="s">
@@ -3536,24 +3542,24 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="17" thickBot="1">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="43">
         <v>2</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="43">
         <v>5</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="43">
         <v>3</v>
       </c>
-      <c r="H6" s="64"/>
-      <c r="I6" s="48">
+      <c r="H6" s="65"/>
+      <c r="I6" s="49">
         <f>SUMPRODUCT(E6:G6,E4:G4)</f>
         <v>17</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="43">
         <v>15</v>
       </c>
       <c r="R6" s="20" t="s">
@@ -3561,37 +3567,37 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="17" thickBot="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="43">
         <v>2</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="43">
         <v>1</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="43">
         <v>2</v>
       </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="48">
+      <c r="H7" s="65"/>
+      <c r="I7" s="49">
         <f>SUMPRODUCT(E7:G7,E4:G4)</f>
         <v>9</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="43">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
       <c r="P8" s="17" t="s">
         <v>17</v>
       </c>
@@ -3600,7 +3606,7 @@
       </c>
     </row>
     <row r="9" spans="1:22">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="40" t="s">
         <v>87</v>
       </c>
       <c r="P9" s="21" t="s">
@@ -3653,7 +3659,7 @@
       <c r="T15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="V15" s="69" t="s">
+      <c r="V15" s="70" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3728,10 +3734,10 @@
       </c>
     </row>
     <row r="21" spans="14:22" ht="17" thickBot="1">
-      <c r="N21" s="67" t="s">
+      <c r="N21" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="P21" s="68" t="s">
+      <c r="P21" s="69" t="s">
         <v>108</v>
       </c>
       <c r="T21" s="20" t="s">
@@ -3742,7 +3748,7 @@
       </c>
     </row>
     <row r="22" spans="14:22">
-      <c r="V22" s="70" t="s">
+      <c r="V22" s="71" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3828,14 +3834,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D490FA9-758B-DC4C-B261-6C467E6A72CA}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="13" max="13" width="5.83203125" customWidth="1"/>
     <col min="14" max="14" width="18.83203125" style="9" customWidth="1"/>
     <col min="15" max="15" width="2.83203125" style="9" customWidth="1"/>
     <col min="16" max="16" width="18.83203125" style="9" customWidth="1"/>
@@ -3845,301 +3852,328 @@
     <col min="20" max="20" width="18.83203125" style="9" customWidth="1"/>
     <col min="21" max="21" width="2.83203125" customWidth="1"/>
     <col min="22" max="22" width="18.83203125" style="9" customWidth="1"/>
+    <col min="23" max="23" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17" thickBot="1">
-      <c r="A1" s="39"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="I1" s="40" t="s">
+    <row r="1" spans="1:20" ht="17" thickBot="1">
+      <c r="A1" s="40"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="I1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="41">
+      <c r="J1" s="42">
         <f>SUMPRODUCT(E2:G2,E5:G5)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:20">
+      <c r="A2" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="43">
         <v>2</v>
       </c>
-      <c r="F2" s="42">
+      <c r="F2" s="43">
         <v>3</v>
       </c>
-      <c r="G2" s="42">
+      <c r="G2" s="43">
         <v>5</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="R2" s="71" t="s">
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="R2" s="72" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="39"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
+    <row r="3" spans="1:20">
+      <c r="A3" s="40"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
       <c r="R3" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
-      <c r="E4" s="42" t="s">
+    <row r="4" spans="1:20">
+      <c r="E4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="42" t="s">
+      <c r="H4" s="65"/>
+      <c r="I4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="43" t="s">
         <v>12</v>
       </c>
       <c r="R4" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="44">
         <v>2</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="44">
         <v>3</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="44">
         <v>0</v>
       </c>
-      <c r="H5" s="64"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
       <c r="R5" s="21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17" thickBot="1">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:20" ht="17" thickBot="1">
+      <c r="A6" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="43">
         <v>1</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="43">
         <v>2</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="43">
         <v>3</v>
       </c>
-      <c r="H6" s="64"/>
+      <c r="H6" s="65"/>
       <c r="I6" s="9">
         <f>SUMPRODUCT(E6:G6,E5:G5)</f>
         <v>8</v>
       </c>
-      <c r="J6" s="64">
+      <c r="J6" s="65">
         <v>7</v>
       </c>
       <c r="R6" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="17" thickBot="1">
-      <c r="A7" s="39" t="s">
+    <row r="7" spans="1:20">
+      <c r="A7" s="40"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="65"/>
+      <c r="R7" s="35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="17" thickBot="1">
+      <c r="A8" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E8" s="43">
         <v>3</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F8" s="43">
         <v>2</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G8" s="43">
         <v>3</v>
       </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="48">
-        <f>SUMPRODUCT(E7:G7,E5:G5)</f>
+      <c r="H8" s="65"/>
+      <c r="I8" s="49">
+        <f>SUMPRODUCT(E8:G8,E5:G5)</f>
         <v>12</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J8" s="43">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="39" t="s">
+    <row r="9" spans="1:20">
+      <c r="A9" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="42"/>
-      <c r="P8" s="17" t="s">
+      <c r="H9" s="65"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="43"/>
+      <c r="P9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="T8" s="17" t="s">
+      <c r="T9" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="39" t="s">
+    <row r="10" spans="1:20">
+      <c r="A10" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="P9" s="21" t="s">
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="P10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="T10" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="39"/>
-      <c r="P10" s="18" t="s">
+    <row r="11" spans="1:20">
+      <c r="A11" s="40"/>
+      <c r="P11" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T10" s="18" t="s">
+      <c r="T11" s="18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
-      <c r="P11" s="18" t="s">
+    <row r="12" spans="1:20">
+      <c r="P12" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="T11" s="19" t="s">
+      <c r="T12" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
-      <c r="P12" s="18" t="s">
+    <row r="13" spans="1:20">
+      <c r="P13" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="T12" s="18" t="s">
+      <c r="T13" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="17" thickBot="1">
-      <c r="P13" s="72" t="s">
+    <row r="14" spans="1:20" ht="17" thickBot="1">
+      <c r="P14" s="73" t="s">
         <v>130</v>
       </c>
-      <c r="T13" s="20" t="s">
+      <c r="T14" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="17" thickBot="1"/>
-    <row r="16" spans="1:22">
-      <c r="N16" s="71" t="s">
+    <row r="16" spans="1:20" ht="17" thickBot="1"/>
+    <row r="17" spans="14:22">
+      <c r="N17" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="P16" s="71" t="s">
+      <c r="P17" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="T16" s="17" t="s">
+      <c r="T17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="V16" s="17" t="s">
+      <c r="V17" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="14:22">
-      <c r="N17" s="19" t="s">
+    <row r="18" spans="14:22">
+      <c r="N18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="19" t="s">
+      <c r="P18" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="T17" s="19" t="s">
+      <c r="T18" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="V17" s="19" t="s">
+      <c r="V18" s="19" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="14:22">
-      <c r="N18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="P18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="T18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="V18" s="11" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="14:22">
       <c r="N19" s="11" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="P19" s="11" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="T19" s="11" t="s">
-        <v>135</v>
+        <v>42</v>
       </c>
       <c r="V19" s="11" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="14:22">
       <c r="N20" s="11" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="P20" s="11" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="14:22">
       <c r="N21" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="T21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="V21" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="14:22">
+      <c r="N22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P21" s="11" t="s">
+      <c r="P22" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="T21" s="11" t="s">
+      <c r="T22" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="V21" s="11" t="s">
+      <c r="V22" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="14:22" ht="17" thickBot="1">
-      <c r="N22" s="12" t="s">
+    <row r="23" spans="14:22" ht="17" thickBot="1">
+      <c r="N23" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P22" s="12" t="s">
+      <c r="P23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="T22" s="12" t="s">
+      <c r="T23" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="V22" s="12" t="s">
+      <c r="V23" s="12" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="14:22">
+      <c r="N24" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="T24" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="V24" s="9" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>